<commit_message>
Total flowchart After update double&int
</commit_message>
<xml_diff>
--- a/two.xlsx
+++ b/two.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$F$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Hub Plant</t>
   </si>
@@ -48,15 +48,6 @@
   </si>
   <si>
     <t>AEC1</t>
-  </si>
-  <si>
-    <t>AEC2</t>
-  </si>
-  <si>
-    <t>AEC3</t>
-  </si>
-  <si>
-    <t>AEC4</t>
   </si>
   <si>
     <t>AED1</t>
@@ -458,7 +449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +458,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,12 +469,12 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11.28515625" customWidth="1"/>
+    <col min="4" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="3">
@@ -493,19 +484,10 @@
         <v>125</v>
       </c>
       <c r="F1" s="3">
-        <v>150</v>
-      </c>
-      <c r="G1" s="3">
-        <v>175</v>
-      </c>
-      <c r="H1" s="3">
-        <v>200</v>
-      </c>
-      <c r="I1" s="3">
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -522,17 +504,8 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -549,24 +522,15 @@
         <v>21000</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5">
         <v>520</v>
@@ -580,22 +544,13 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="2">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
         <v>362</v>
@@ -607,20 +562,11 @@
         <v>2</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
         <v>400</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:I5"/>
+  <autoFilter ref="A2:F5"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -631,23 +577,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Customer_x0020_Name xmlns="dab2140f-ee56-48f7-9b1b-e1b14801fef8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDD8E62889A3946A4E18A918E574D11" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fd5446997075c2330ea4d1053980c75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dab2140f-ee56-48f7-9b1b-e1b14801fef8" xmlns:ns3="792410c9-d2d1-4be9-81e4-5b58d42acfec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e94a531d836e9fec5905c03634bf0da9" ns2:_="" ns3:_="">
     <xsd:import namespace="dab2140f-ee56-48f7-9b1b-e1b14801fef8"/>
@@ -858,25 +787,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Customer_x0020_Name xmlns="dab2140f-ee56-48f7-9b1b-e1b14801fef8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0F95189-0F5B-458B-AE56-687279E76256}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dab2140f-ee56-48f7-9b1b-e1b14801fef8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA3C5E04-DC86-48FD-AF76-4D2CD543C7A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B109A25E-271D-41A8-A5F3-CF894BAEAA51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -893,4 +821,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA3C5E04-DC86-48FD-AF76-4D2CD543C7A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0F95189-0F5B-458B-AE56-687279E76256}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dab2140f-ee56-48f7-9b1b-e1b14801fef8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>